<commit_message>
Ya funciona el limpiador de la base de datos
</commit_message>
<xml_diff>
--- a/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
+++ b/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/b_riverah_uniandes_edu_co/Documents/SISTRANS_proyecto/enunciados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/b_riverah_uniandes_edu_co/Documents/D-11/SISTRANS-PROYECTO/enunciados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5ECEFBC-81E5-4716-88D5-F2282824185C}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63E33733-05E3-4E58-8B19-B3B0463A153D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="172">
   <si>
     <t>Relación</t>
   </si>
@@ -375,9 +375,6 @@
     <t>FK Estilo.idEstilo</t>
   </si>
   <si>
-    <t>FK HorarioServicio.idHorarioServicio</t>
-  </si>
-  <si>
     <t>CartaProductos</t>
   </si>
   <si>
@@ -538,6 +535,12 @@
   </si>
   <si>
     <t>contraseña</t>
+  </si>
+  <si>
+    <t>descripción</t>
+  </si>
+  <si>
+    <t>profundidad</t>
   </si>
 </sst>
 </file>
@@ -968,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FN366"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3460,7 +3463,7 @@
         <v>50</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -8451,7 +8454,7 @@
     <row r="43" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
@@ -9513,11 +9516,9 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="4" t="s">
+      <c r="G49" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
@@ -9690,15 +9691,15 @@
       <c r="C50" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="6" t="s">
+      <c r="D50" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
@@ -9868,15 +9869,15 @@
       <c r="C51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
@@ -10046,15 +10047,15 @@
       <c r="C52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="8" t="s">
+      <c r="D52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="H52" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
@@ -10753,7 +10754,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="2" t="s">
@@ -12675,7 +12676,7 @@
         <v>93</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>16</v>
@@ -15168,12 +15169,12 @@
         <v>112</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
-      <c r="M81" s="10"/>
+      <c r="M81" s="4"/>
       <c r="N81" s="4"/>
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
@@ -15330,9 +15331,8 @@
       <c r="FK81" s="4"/>
       <c r="FL81" s="4"/>
       <c r="FM81" s="4"/>
-      <c r="FN81" s="4"/>
     </row>
-    <row r="82" spans="1:170" ht="66" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A82" s="4"/>
       <c r="B82" s="2" t="s">
         <v>15</v>
@@ -15364,9 +15364,7 @@
       <c r="K82" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="L82" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="L82" s="2"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
       <c r="O82" s="4"/>
@@ -15524,7 +15522,6 @@
       <c r="FK82" s="4"/>
       <c r="FL82" s="4"/>
       <c r="FM82" s="4"/>
-      <c r="FN82" s="4"/>
     </row>
     <row r="83" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A83" s="4"/>
@@ -15559,7 +15556,7 @@
         <v>18</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
@@ -15718,7 +15715,6 @@
       <c r="FK83" s="4"/>
       <c r="FL83" s="4"/>
       <c r="FM83" s="4"/>
-      <c r="FN83" s="4"/>
     </row>
     <row r="84" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
@@ -16067,7 +16063,7 @@
     <row r="86" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A86" s="4"/>
       <c r="B86" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -16245,24 +16241,24 @@
     <row r="87" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A87" s="4"/>
       <c r="B87" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C87" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J87" s="6" t="s">
         <v>42</v>
@@ -17144,7 +17140,7 @@
     <row r="92" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -17156,7 +17152,7 @@
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
       <c r="J92" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
@@ -17322,7 +17318,7 @@
     <row r="93" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>26</v>
@@ -17335,32 +17331,32 @@
       </c>
       <c r="F93" s="10"/>
       <c r="G93" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I93" s="4"/>
       <c r="J93" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K93" s="6" t="s">
         <v>26</v>
       </c>
       <c r="L93" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="M93" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="M93" s="6" t="s">
+      <c r="N93" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="N93" s="6" t="s">
+      <c r="O93" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="O93" s="6" t="s">
-        <v>130</v>
-      </c>
       <c r="P93" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q93" s="10"/>
       <c r="R93" s="4"/>
@@ -17550,7 +17546,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="2"/>
       <c r="P94" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
@@ -17917,7 +17913,7 @@
       <c r="M96" s="4"/>
       <c r="N96" s="4"/>
       <c r="O96" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>
@@ -18250,7 +18246,7 @@
     <row r="98" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A98" s="4"/>
       <c r="B98" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
@@ -18267,7 +18263,7 @@
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
       <c r="O98" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P98" s="4"/>
       <c r="Q98" s="4"/>
@@ -18428,20 +18424,20 @@
     <row r="99" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A99" s="4"/>
       <c r="B99" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C99" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G99" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H99" s="10"/>
       <c r="I99" s="4"/>
@@ -18623,7 +18619,7 @@
         <v>16</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
@@ -19318,22 +19314,22 @@
     <row r="104" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A104" s="4"/>
       <c r="B104" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
       <c r="K104" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L104" s="4"/>
       <c r="M104" s="4"/>
@@ -19498,31 +19494,31 @@
     <row r="105" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A105" s="4"/>
       <c r="B105" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>92</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I105" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J105" s="4"/>
       <c r="K105" s="6" t="s">
         <v>104</v>
       </c>
       <c r="L105" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M105" s="10"/>
       <c r="N105" s="4"/>
@@ -19689,18 +19685,18 @@
         <v>103</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>93</v>
@@ -19710,7 +19706,7 @@
         <v>103</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M106" s="10"/>
       <c r="N106" s="4"/>
@@ -20406,22 +20402,22 @@
     <row r="110" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A110" s="4"/>
       <c r="B110" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I110" s="4"/>
       <c r="J110" s="4"/>
       <c r="K110" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L110" s="4"/>
       <c r="M110" s="12"/>
@@ -20600,7 +20596,7 @@
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I111" s="6" t="s">
         <v>104</v>
@@ -20774,31 +20770,31 @@
     <row r="112" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A112" s="4"/>
       <c r="B112" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G112" s="4"/>
       <c r="H112" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I112" s="2" t="s">
         <v>103</v>
       </c>
       <c r="J112" s="4"/>
       <c r="K112" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M112" s="10"/>
       <c r="N112" s="4"/>
@@ -21494,22 +21490,22 @@
     <row r="116" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A116" s="4"/>
       <c r="B116" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F116" s="4"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I116" s="4"/>
       <c r="J116" s="4"/>
       <c r="K116" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L116" s="4"/>
       <c r="M116" s="12"/>
@@ -21674,31 +21670,31 @@
     <row r="117" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A117" s="4"/>
       <c r="B117" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="6" t="s">
         <v>21</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G117" s="4"/>
       <c r="H117" s="6" t="s">
         <v>78</v>
       </c>
       <c r="I117" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J117" s="4"/>
       <c r="K117" s="6" t="s">
         <v>66</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M117" s="10"/>
       <c r="N117" s="4"/>
@@ -21862,31 +21858,31 @@
     <row r="118" spans="1:170" ht="66" x14ac:dyDescent="0.3">
       <c r="A118" s="4"/>
       <c r="B118" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G118" s="4"/>
       <c r="H118" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J118" s="4"/>
       <c r="K118" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M118" s="10"/>
       <c r="N118" s="4"/>

</xml_diff>

<commit_message>
funcionando hasta req funcional 7
</commit_message>
<xml_diff>
--- a/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
+++ b/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/b_riverah_uniandes_edu_co/Documents/D-11/SISTRANS-PROYECTO/enunciados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63E33733-05E3-4E58-8B19-B3B0463A153D}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DF365D6-CCEC-4E9C-91D2-8D82FDE11A48}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla Relación" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="173">
   <si>
     <t>Relación</t>
   </si>
@@ -542,6 +542,9 @@
   <si>
     <t>profundidad</t>
   </si>
+  <si>
+    <t>NN,FK Servicio.idServicio</t>
+  </si>
 </sst>
 </file>
 
@@ -971,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FN366"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A77" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5611,12 +5614,10 @@
         <v>14</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="M27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -5773,7 +5774,6 @@
       <c r="FK27" s="4"/>
       <c r="FL27" s="4"/>
       <c r="FM27" s="4"/>
-      <c r="FN27" s="4"/>
     </row>
     <row r="28" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
@@ -5799,11 +5799,9 @@
         <v>17</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L28" s="2" t="s">
         <v>85</v>
       </c>
+      <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -5961,7 +5959,6 @@
       <c r="FK28" s="4"/>
       <c r="FL28" s="4"/>
       <c r="FM28" s="4"/>
-      <c r="FN28" s="4"/>
     </row>
     <row r="29" spans="1:170" ht="33" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
@@ -5995,9 +5992,7 @@
       <c r="K29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L29" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -6155,7 +6150,6 @@
       <c r="FK29" s="4"/>
       <c r="FL29" s="4"/>
       <c r="FM29" s="4"/>
-      <c r="FN29" s="4"/>
     </row>
     <row r="30" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
@@ -11457,10 +11451,9 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="4" t="s">
+      <c r="G60" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G60" s="4"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
@@ -11633,11 +11626,12 @@
       <c r="D61" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="6" t="s">
+      <c r="E61" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G61" s="4"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -11797,8 +11791,8 @@
       <c r="FK61" s="4"/>
       <c r="FL61" s="4"/>
     </row>
-    <row r="62" spans="1:170" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+    <row r="62" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A62" s="10"/>
       <c r="B62" s="2" t="s">
         <v>15</v>
       </c>
@@ -11808,11 +11802,12 @@
       <c r="D62" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="2" t="s">
+      <c r="E62" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G62" s="4"/>
       <c r="K62" s="4"/>
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
@@ -11983,11 +11978,12 @@
       <c r="D63" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E63" s="4"/>
-      <c r="F63" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="4"/>
+      <c r="G63" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="K63" s="4"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>

</xml_diff>

<commit_message>
Hasta req funcional 7 funcionando sin problemas
</commit_message>
<xml_diff>
--- a/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
+++ b/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/b_riverah_uniandes_edu_co/Documents/D-11/SISTRANS-PROYECTO/enunciados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DF365D6-CCEC-4E9C-91D2-8D82FDE11A48}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E1095CE-28B6-49C2-9FB1-1486B7971A8A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="173">
   <si>
     <t>Relación</t>
   </si>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FN366"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5616,7 +5616,9 @@
       <c r="K27" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="L27" s="10"/>
+      <c r="L27" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -5801,7 +5803,9 @@
       <c r="K28" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L28" s="4"/>
+      <c r="L28" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -5992,7 +5996,9 @@
       <c r="K29" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L29" s="4"/>
+      <c r="L29" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>

</xml_diff>

<commit_message>
Hasta req funcional 9 sirviendo**
</commit_message>
<xml_diff>
--- a/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
+++ b/SISTRANS-PROYECTO/enunciados/isis2304-Plantilla Relación (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/b_riverah_uniandes_edu_co/Documents/D-11/SISTRANS-PROYECTO/enunciados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E1095CE-28B6-49C2-9FB1-1486B7971A8A}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{663AA640-F4F0-478B-AA5F-F492E541B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04004BC0-24B3-4B8F-AA4B-4A83F63C1C62}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="174">
   <si>
     <t>Relación</t>
   </si>
@@ -545,6 +545,9 @@
   <si>
     <t>NN,FK Servicio.idServicio</t>
   </si>
+  <si>
+    <t>NN,FK Cuenta.idCuenta</t>
+  </si>
 </sst>
 </file>
 
@@ -583,7 +586,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,12 +622,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -655,7 +652,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -687,8 +684,14 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -974,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FN366"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2558,7 +2561,6 @@
       <c r="FK9" s="4"/>
       <c r="FL9" s="4"/>
       <c r="FM9" s="4"/>
-      <c r="FN9" s="4"/>
     </row>
     <row r="10" spans="1:170" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -2572,7 +2574,7 @@
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -2736,7 +2738,6 @@
       <c r="FK10" s="4"/>
       <c r="FL10" s="4"/>
       <c r="FM10" s="4"/>
-      <c r="FN10" s="4"/>
     </row>
     <row r="11" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
@@ -2916,7 +2917,6 @@
       <c r="FK11" s="4"/>
       <c r="FL11" s="4"/>
       <c r="FM11" s="4"/>
-      <c r="FN11" s="4"/>
     </row>
     <row r="12" spans="1:170" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
@@ -6520,8 +6520,9 @@
       <c r="F32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
+      <c r="G32" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -6702,8 +6703,9 @@
       <c r="F33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G33" s="10"/>
-      <c r="H33" s="4"/>
+      <c r="G33" s="13" t="s">
+        <v>173</v>
+      </c>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -6884,8 +6886,9 @@
       <c r="F34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
+      <c r="G34" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>

</xml_diff>